<commit_message>
chore: update pcb for smt
</commit_message>
<xml_diff>
--- a/assets/BOM.xlsx
+++ b/assets/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B81B9D-8D1A-4FC8-B4B1-BACADFA27FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4691D65A-32C3-45DB-98B3-5AA6302B6788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="12835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="172">
   <si>
     <t>No.</t>
   </si>
@@ -519,6 +519,18 @@
   </si>
   <si>
     <t>1.1A</t>
+  </si>
+  <si>
+    <t>4.7V</t>
+  </si>
+  <si>
+    <t>15V</t>
+  </si>
+  <si>
+    <t>4.3V</t>
+  </si>
+  <si>
+    <t>For manual assembly</t>
   </si>
 </sst>
 </file>
@@ -563,12 +575,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -910,15 +925,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.77734375" customWidth="1"/>
+    <col min="1" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1703,7 +1720,7 @@
         <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="F25" t="s">
         <v>136</v>
@@ -1735,7 +1752,7 @@
         <v>135</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>169</v>
       </c>
       <c r="F26" t="s">
         <v>140</v>
@@ -1767,7 +1784,7 @@
         <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="F27" t="s">
         <v>144</v>
@@ -1789,11 +1806,14 @@
       <c r="A28" t="s">
         <v>146</v>
       </c>
-      <c r="B28" t="s">
-        <v>147</v>
+      <c r="B28" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>147</v>
       </c>
       <c r="F28" t="s">
         <v>148</v>
@@ -1806,11 +1826,12 @@
       <c r="A29" t="s">
         <v>150</v>
       </c>
-      <c r="B29" t="s">
-        <v>151</v>
-      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="1">
         <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>151</v>
       </c>
       <c r="F29" t="s">
         <v>152</v>
@@ -1823,11 +1844,12 @@
       <c r="A30" t="s">
         <v>153</v>
       </c>
-      <c r="B30" t="s">
-        <v>154</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="1">
         <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>154</v>
       </c>
       <c r="F30" t="s">
         <v>155</v>
@@ -1840,11 +1862,12 @@
       <c r="A31" t="s">
         <v>156</v>
       </c>
-      <c r="B31" t="s">
-        <v>157</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="1">
         <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>157</v>
       </c>
       <c r="F31" t="s">
         <v>158</v>
@@ -1857,11 +1880,12 @@
       <c r="A32" t="s">
         <v>159</v>
       </c>
-      <c r="B32" t="s">
-        <v>160</v>
-      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="1">
         <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
       </c>
       <c r="F32" t="s">
         <v>161</v>
@@ -1877,12 +1901,13 @@
       <c r="A33" t="s">
         <v>163</v>
       </c>
-      <c r="B33" t="s">
-        <v>164</v>
-      </c>
+      <c r="B33" s="3"/>
       <c r="C33" s="1">
         <v>1</v>
       </c>
+      <c r="D33" t="s">
+        <v>164</v>
+      </c>
       <c r="F33" t="s">
         <v>165</v>
       </c>
@@ -1891,8 +1916,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B28:B33"/>
+  </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>